<commit_message>
measurement 제외조건 수정, visit_detail제외조건 추가
</commit_message>
<xml_diff>
--- a/JBUH/감염병_CDM_ETL정의서.xlsx
+++ b/JBUH/감염병_CDM_ETL정의서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programing\Infectious_CDM\JBUH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA7C4E9-794B-4EB3-8E2A-B4A2F560899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAD1209-C643-4037-B008-DF9E6A0587B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" tabRatio="855" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" tabRatio="855" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCATION" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="794">
   <si>
     <t>필드명</t>
   </si>
@@ -3070,6 +3070,27 @@
   </si>
   <si>
     <t>병동번호에 해당하는 명칭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>병동번호에 해당하는 데이터만 포함
+deptcode deptlnm
+1002 ICU(본관중환자실)
+1003 외과계중환자실(SICU)
+1004 MICU(내과계중환자실)_사용안함
+1005 신생아집중치료실(NICU)
+2002 신경계중환자실(NCU)
+2003 응급전용중환자실(EICU)
+2004 내과계중환자실(MICU)
+2007 EICU(MICU임시)
+2008 심장계중환자실(CCU)
+5002 소아집중치료실(PICU)
+5004 산모태아집중치료실(MFICU)
+6002 SUB-ICU
+ICU1 본관중환자실1
+ICU2 본관중환자실2
+ICU3 본관중환자실3
+SI 외과중환자실</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3411,7 +3432,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3598,31 +3619,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4513,7 +4510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -4688,49 +4685,49 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" s="70" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="69" t="s">
+    <row r="8" spans="1:8" s="14" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="E8" s="67" t="s">
+      <c r="E8" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="13" t="s">
         <v>788</v>
       </c>
-      <c r="H8" s="62"/>
-    </row>
-    <row r="9" spans="1:8" s="70" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="69" t="s">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="13" t="s">
         <v>788</v>
       </c>
-      <c r="H9" s="62"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -9374,8 +9371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4475453-F8A9-444B-9F7E-F19D36EE47F7}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9668,278 +9665,278 @@
         <v>531</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="62" t="s">
         <v>311</v>
       </c>
-      <c r="F14" s="64" t="s">
+      <c r="F14" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="G14" s="65" t="s">
+      <c r="G14" s="13" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E15" s="67" t="s">
+      <c r="E15" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="65" t="s">
+      <c r="F15" s="19"/>
+      <c r="G15" s="13" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="62" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="1" t="s">
         <v>762</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="G16" s="65" t="s">
+      <c r="G16" s="13" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="62" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E17" s="68" t="s">
+      <c r="E17" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65" t="s">
+      <c r="F17" s="19"/>
+      <c r="G17" s="13" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E18" s="68" t="s">
+      <c r="E18" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="13" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="62" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="68" t="s">
+      <c r="D19" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="E19" s="67" t="s">
+      <c r="E19" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="F19" s="64"/>
-      <c r="G19" s="65" t="s">
+      <c r="F19" s="19"/>
+      <c r="G19" s="13" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="66" customFormat="1" ht="27" x14ac:dyDescent="0.3">
-      <c r="A20" s="62" t="s">
+    <row r="20" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="F20" s="64" t="s">
+      <c r="F20" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="G20" s="65" t="s">
+      <c r="G20" s="13" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="62" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="F21" s="64"/>
-      <c r="G21" s="65" t="s">
+      <c r="F21" s="19"/>
+      <c r="G21" s="13" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="62" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E22" s="68" t="s">
+      <c r="E22" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="19" t="s">
         <v>361</v>
       </c>
-      <c r="G22" s="65" t="s">
+      <c r="G22" s="13" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="69" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>784</v>
       </c>
-      <c r="E23" s="62" t="s">
+      <c r="E23" s="2" t="s">
         <v>784</v>
       </c>
-      <c r="F23" s="64" t="s">
+      <c r="F23" s="19" t="s">
         <v>452</v>
       </c>
-      <c r="G23" s="62" t="s">
+      <c r="G23" s="2" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="69" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>785</v>
       </c>
-      <c r="E24" s="62" t="s">
+      <c r="E24" s="2" t="s">
         <v>785</v>
       </c>
-      <c r="F24" s="62" t="s">
+      <c r="F24" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="G24" s="62" t="s">
+      <c r="G24" s="2" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="62" t="s">
+    <row r="25" spans="1:7" ht="243" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>786</v>
       </c>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="2" t="s">
         <v>791</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
         <v>786</v>
       </c>
-      <c r="E25" s="62" t="s">
-        <v>786</v>
-      </c>
-      <c r="F25" s="62" t="s">
+      <c r="E25" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="G25" s="62" t="s">
+      <c r="G25" s="2" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="62" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="2" t="s">
         <v>791</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="E26" s="62" t="s">
+      <c r="E26" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="F26" s="62" t="s">
+      <c r="F26" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="G26" s="62" t="s">
+      <c r="G26" s="2" t="s">
         <v>790</v>
       </c>
     </row>

</xml_diff>

<commit_message>
drug_exposure_end_date 계산식 변경, ETL정의서 반영, KNUH measurement_pth조건 수정
</commit_message>
<xml_diff>
--- a/JBUH/감염병_CDM_ETL정의서.xlsx
+++ b/JBUH/감염병_CDM_ETL정의서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programing\Infectious_CDM\JBUH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAD1209-C643-4037-B008-DF9E6A0587B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E239D1D-858B-4CAE-9693-6D20A7D2DC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" tabRatio="855" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="855" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCATION" sheetId="2" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="794">
   <si>
     <t>필드명</t>
   </si>
@@ -3051,10 +3051,6 @@
   </si>
   <si>
     <t>WARDNO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORDDATE + DAY</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -3091,6 +3087,10 @@
 ICU2 본관중환자실2
 ICU3 본관중환자실3
 SI 외과중환자실</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORDDATE + DAY - 1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4510,8 +4510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4703,7 +4703,7 @@
         <v>476</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>788</v>
+        <v>793</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -4725,7 +4725,7 @@
         <v>476</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>788</v>
+        <v>793</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -9371,7 +9371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4475453-F8A9-444B-9F7E-F19D36EE47F7}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -9903,14 +9903,14 @@
         <v>786</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>786</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>364</v>
@@ -9921,23 +9921,23 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>779</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>